<commit_message>
엑셀 및 Json 데이터 추가 (Object, Trophy 포함)
</commit_message>
<xml_diff>
--- a/Excel/EposTileInfo.xlsx
+++ b/Excel/EposTileInfo.xlsx
@@ -3,8 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Tile" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sub_Idea" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="시트3" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Tile" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Sub_Idea" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -44,52 +45,52 @@
     <t>5TierPattern</t>
   </si>
   <si>
+    <t>TierTile4Model</t>
+  </si>
+  <si>
+    <t>4TierPattern</t>
+  </si>
+  <si>
+    <t>TierTile3Model</t>
+  </si>
+  <si>
+    <t>3TierPattern</t>
+  </si>
+  <si>
+    <t>TierTile2Model</t>
+  </si>
+  <si>
+    <t>2TierPattern</t>
+  </si>
+  <si>
+    <t>TierTile1Model</t>
+  </si>
+  <si>
+    <t>1TierPattern</t>
+  </si>
+  <si>
+    <t>BlankTile</t>
+  </si>
+  <si>
+    <t>BlankTileModel</t>
+  </si>
+  <si>
+    <t>BlankPattern</t>
+  </si>
+  <si>
+    <t>InteractionTile</t>
+  </si>
+  <si>
+    <t>InteractionTileModel</t>
+  </si>
+  <si>
+    <t>EnvironmentTile</t>
+  </si>
+  <si>
+    <t>EnvironmentTileModel</t>
+  </si>
+  <si>
     <t>TileInfo</t>
-  </si>
-  <si>
-    <t>TierTile4Model</t>
-  </si>
-  <si>
-    <t>4TierPattern</t>
-  </si>
-  <si>
-    <t>TierTile3Model</t>
-  </si>
-  <si>
-    <t>3TierPattern</t>
-  </si>
-  <si>
-    <t>TierTile2Model</t>
-  </si>
-  <si>
-    <t>2TierPattern</t>
-  </si>
-  <si>
-    <t>TierTile1Model</t>
-  </si>
-  <si>
-    <t>1TierPattern</t>
-  </si>
-  <si>
-    <t>BlankTile</t>
-  </si>
-  <si>
-    <t>BlankTileModel</t>
-  </si>
-  <si>
-    <t>BlankPattern</t>
-  </si>
-  <si>
-    <t>InteractionTile</t>
-  </si>
-  <si>
-    <t>InteractionTileModel</t>
-  </si>
-  <si>
-    <t>EnvironmentTile</t>
-  </si>
-  <si>
-    <t>EnvironmentTileModel</t>
   </si>
   <si>
     <t>ItemRate</t>
@@ -370,14 +371,14 @@
       <name val="&quot;맑은 고딕&quot;"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="6">
@@ -442,11 +443,11 @@
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -473,6 +474,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -679,6 +684,199 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>101.0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <f t="shared" ref="A3:A10" si="1">A2+1</f>
+        <v>102</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="20.75"/>
     <col customWidth="1" min="3" max="3" width="22.13"/>
@@ -704,676 +902,619 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2">
-        <v>101.0</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="Y3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="K64" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="F65" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M65" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="N65" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q65" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R65" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T65" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V65" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X65" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="F66" s="2">
+        <v>9010001.0</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H66" s="2">
         <v>10.0</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <f t="shared" ref="A5:A12" si="1">A4+1</f>
-        <v>102</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="I66" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K66" s="2">
+        <v>1070001.0</v>
+      </c>
+      <c r="L66" s="2">
+        <v>1030006.0</v>
+      </c>
+      <c r="M66" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="N66" s="2">
+        <v>1050001.0</v>
+      </c>
+      <c r="O66" s="2">
+        <f t="shared" ref="O66:O71" si="1">10000/5</f>
+        <v>2000</v>
+      </c>
+      <c r="P66" s="2">
+        <v>1050002.0</v>
+      </c>
+      <c r="Q66" s="2">
+        <f t="shared" ref="Q66:Q71" si="2">10000/5</f>
+        <v>2000</v>
+      </c>
+      <c r="R66" s="2">
+        <v>1050003.0</v>
+      </c>
+      <c r="S66" s="2">
+        <f t="shared" ref="S66:S71" si="3">10000/5</f>
+        <v>2000</v>
+      </c>
+      <c r="T66" s="2">
+        <v>1050003.0</v>
+      </c>
+      <c r="U66" s="2">
+        <f t="shared" ref="U66:U71" si="4">10000/5</f>
+        <v>2000</v>
+      </c>
+      <c r="V66" s="2">
+        <v>1050005.0</v>
+      </c>
+      <c r="W66" s="2">
+        <f t="shared" ref="W66:W71" si="5">10000/5</f>
+        <v>2000</v>
+      </c>
+      <c r="X66" s="2">
+        <f t="shared" ref="X66:X77" si="6">SUM(W66,U66,S66,Q66,O66)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="F67" s="2">
+        <f t="shared" ref="F67:F73" si="7">F66+1</f>
+        <v>9010002</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H67" s="2">
         <v>20.0</v>
       </c>
-      <c r="Y5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2">
+      <c r="I67" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K67" s="2">
+        <f t="shared" ref="K67:K77" si="8">K66+1</f>
+        <v>1070002</v>
+      </c>
+      <c r="L67" s="2">
+        <v>1030007.0</v>
+      </c>
+      <c r="M67" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="N67" s="2">
+        <v>1050001.0</v>
+      </c>
+      <c r="O67" s="2">
         <f t="shared" si="1"/>
-        <v>103</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2">
-        <v>40.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="2">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2">
-        <f t="shared" si="1"/>
-        <v>106</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="2">
-        <v>60.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2">
-        <f t="shared" si="1"/>
-        <v>107</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2">
-        <f t="shared" si="1"/>
-        <v>108</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2">
-        <f t="shared" si="1"/>
-        <v>109</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="K66" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="F67" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K67" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L67" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M67" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N67" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O67" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P67" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q67" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R67" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S67" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T67" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="U67" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V67" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W67" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X67" s="5" t="s">
-        <v>43</v>
+        <v>2000</v>
+      </c>
+      <c r="P67" s="2">
+        <v>1050002.0</v>
+      </c>
+      <c r="Q67" s="2">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="R67" s="2">
+        <v>1050003.0</v>
+      </c>
+      <c r="S67" s="2">
+        <f t="shared" si="3"/>
+        <v>2000</v>
+      </c>
+      <c r="T67" s="2">
+        <v>1050003.0</v>
+      </c>
+      <c r="U67" s="2">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="V67" s="2">
+        <v>1050005.0</v>
+      </c>
+      <c r="W67" s="2">
+        <f t="shared" si="5"/>
+        <v>2000</v>
+      </c>
+      <c r="X67" s="2">
+        <f t="shared" si="6"/>
+        <v>10000</v>
       </c>
     </row>
     <row r="68">
       <c r="F68" s="2">
-        <v>9010001.0</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>44</v>
+        <f t="shared" si="7"/>
+        <v>9010003</v>
+      </c>
+      <c r="G68" s="2">
+        <v>0.0</v>
       </c>
       <c r="H68" s="2">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="I68" s="2">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="K68" s="2">
-        <v>1070001.0</v>
+        <f t="shared" si="8"/>
+        <v>1070003</v>
       </c>
       <c r="L68" s="2">
-        <v>1030006.0</v>
+        <v>1030008.0</v>
       </c>
       <c r="M68" s="2">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="N68" s="2">
         <v>1050001.0</v>
       </c>
       <c r="O68" s="2">
-        <f t="shared" ref="O68:O73" si="2">10000/5</f>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="P68" s="2">
         <v>1050002.0</v>
       </c>
       <c r="Q68" s="2">
-        <f t="shared" ref="Q68:Q73" si="3">10000/5</f>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="R68" s="2">
         <v>1050003.0</v>
       </c>
       <c r="S68" s="2">
-        <f t="shared" ref="S68:S73" si="4">10000/5</f>
+        <f t="shared" si="3"/>
         <v>2000</v>
       </c>
       <c r="T68" s="2">
         <v>1050003.0</v>
       </c>
       <c r="U68" s="2">
-        <f t="shared" ref="U68:U73" si="5">10000/5</f>
+        <f t="shared" si="4"/>
         <v>2000</v>
       </c>
       <c r="V68" s="2">
         <v>1050005.0</v>
       </c>
       <c r="W68" s="2">
-        <f t="shared" ref="W68:W73" si="6">10000/5</f>
+        <f t="shared" si="5"/>
         <v>2000</v>
       </c>
       <c r="X68" s="2">
-        <f t="shared" ref="X68:X79" si="7">SUM(W68,U68,S68,Q68,O68)</f>
+        <f t="shared" si="6"/>
         <v>10000</v>
       </c>
     </row>
     <row r="69">
       <c r="F69" s="2">
-        <f t="shared" ref="F69:F75" si="8">F68+1</f>
-        <v>9010002</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>44</v>
+        <f t="shared" si="7"/>
+        <v>9010004</v>
+      </c>
+      <c r="G69" s="2">
+        <v>0.0</v>
       </c>
       <c r="H69" s="2">
-        <v>20.0</v>
+        <v>30.0</v>
       </c>
       <c r="I69" s="2">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="K69" s="2">
-        <f t="shared" ref="K69:K79" si="9">K68+1</f>
-        <v>1070002</v>
+        <f t="shared" si="8"/>
+        <v>1070004</v>
       </c>
       <c r="L69" s="2">
-        <v>1030007.0</v>
+        <v>1030009.0</v>
       </c>
       <c r="M69" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="N69" s="2">
         <v>1050001.0</v>
       </c>
       <c r="O69" s="2">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="P69" s="2">
+        <v>1050002.0</v>
+      </c>
+      <c r="Q69" s="2">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
-      <c r="P69" s="2">
-        <v>1050002.0</v>
-      </c>
-      <c r="Q69" s="2">
+      <c r="R69" s="2">
+        <v>1050003.0</v>
+      </c>
+      <c r="S69" s="2">
         <f t="shared" si="3"/>
         <v>2000</v>
       </c>
-      <c r="R69" s="2">
+      <c r="T69" s="2">
         <v>1050003.0</v>
       </c>
-      <c r="S69" s="2">
+      <c r="U69" s="2">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
-      <c r="T69" s="2">
-        <v>1050003.0</v>
-      </c>
-      <c r="U69" s="2">
+      <c r="V69" s="2">
+        <v>1050005.0</v>
+      </c>
+      <c r="W69" s="2">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="V69" s="2">
-        <v>1050005.0</v>
-      </c>
-      <c r="W69" s="2">
+      <c r="X69" s="2">
         <f t="shared" si="6"/>
-        <v>2000</v>
-      </c>
-      <c r="X69" s="2">
-        <f t="shared" si="7"/>
         <v>10000</v>
       </c>
     </row>
     <row r="70">
       <c r="F70" s="2">
+        <f t="shared" si="7"/>
+        <v>9010005</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H70" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="I70" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K70" s="2">
         <f t="shared" si="8"/>
-        <v>9010003</v>
-      </c>
-      <c r="G70" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H70" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="I70" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="K70" s="2">
-        <f t="shared" si="9"/>
-        <v>1070003</v>
+        <v>1070005</v>
       </c>
       <c r="L70" s="2">
-        <v>1030008.0</v>
+        <v>1030010.0</v>
       </c>
       <c r="M70" s="2">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="N70" s="2">
         <v>1050001.0</v>
       </c>
       <c r="O70" s="2">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="P70" s="2">
+        <v>1050002.0</v>
+      </c>
+      <c r="Q70" s="2">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
-      <c r="P70" s="2">
-        <v>1050002.0</v>
-      </c>
-      <c r="Q70" s="2">
+      <c r="R70" s="2">
+        <v>1050003.0</v>
+      </c>
+      <c r="S70" s="2">
         <f t="shared" si="3"/>
         <v>2000</v>
       </c>
-      <c r="R70" s="2">
+      <c r="T70" s="2">
         <v>1050003.0</v>
       </c>
-      <c r="S70" s="2">
+      <c r="U70" s="2">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
-      <c r="T70" s="2">
-        <v>1050003.0</v>
-      </c>
-      <c r="U70" s="2">
+      <c r="V70" s="2">
+        <v>1050005.0</v>
+      </c>
+      <c r="W70" s="2">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="V70" s="2">
-        <v>1050005.0</v>
-      </c>
-      <c r="W70" s="2">
+      <c r="X70" s="2">
         <f t="shared" si="6"/>
-        <v>2000</v>
-      </c>
-      <c r="X70" s="2">
-        <f t="shared" si="7"/>
         <v>10000</v>
       </c>
     </row>
     <row r="71">
       <c r="F71" s="2">
+        <f t="shared" si="7"/>
+        <v>9010006</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H71" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="I71" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K71" s="2">
         <f t="shared" si="8"/>
-        <v>9010004</v>
-      </c>
-      <c r="G71" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="H71" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="I71" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="K71" s="2">
-        <f t="shared" si="9"/>
-        <v>1070004</v>
+        <v>1070006</v>
       </c>
       <c r="L71" s="2">
-        <v>1030009.0</v>
+        <v>1030011.0</v>
       </c>
       <c r="M71" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="N71" s="2">
         <v>1050001.0</v>
       </c>
       <c r="O71" s="2">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="P71" s="2">
+        <v>1050002.0</v>
+      </c>
+      <c r="Q71" s="2">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
-      <c r="P71" s="2">
-        <v>1050002.0</v>
-      </c>
-      <c r="Q71" s="2">
+      <c r="R71" s="2">
+        <v>1050003.0</v>
+      </c>
+      <c r="S71" s="2">
         <f t="shared" si="3"/>
         <v>2000</v>
       </c>
-      <c r="R71" s="2">
+      <c r="T71" s="2">
         <v>1050003.0</v>
       </c>
-      <c r="S71" s="2">
+      <c r="U71" s="2">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
-      <c r="T71" s="2">
-        <v>1050003.0</v>
-      </c>
-      <c r="U71" s="2">
+      <c r="V71" s="2">
+        <v>1050005.0</v>
+      </c>
+      <c r="W71" s="2">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="V71" s="2">
-        <v>1050005.0</v>
-      </c>
-      <c r="W71" s="2">
+      <c r="X71" s="2">
         <f t="shared" si="6"/>
-        <v>2000</v>
-      </c>
-      <c r="X71" s="2">
-        <f t="shared" si="7"/>
         <v>10000</v>
       </c>
     </row>
     <row r="72">
       <c r="F72" s="2">
-        <f t="shared" si="8"/>
-        <v>9010005</v>
+        <f t="shared" si="7"/>
+        <v>9010007</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H72" s="2">
-        <v>50.0</v>
+        <v>20.0</v>
       </c>
       <c r="I72" s="2">
         <v>0.0</v>
       </c>
       <c r="K72" s="2">
-        <f t="shared" si="9"/>
-        <v>1070005</v>
+        <f t="shared" si="8"/>
+        <v>1070007</v>
       </c>
       <c r="L72" s="2">
-        <v>1030010.0</v>
+        <f t="shared" ref="L72:L77" si="9">L71+1</f>
+        <v>1030012</v>
       </c>
       <c r="M72" s="2">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="N72" s="2">
-        <v>1050001.0</v>
-      </c>
-      <c r="O72" s="2">
-        <f t="shared" si="2"/>
-        <v>2000</v>
+        <f t="shared" ref="N72:N77" si="10">N71+1</f>
+        <v>1050002</v>
+      </c>
+      <c r="O72" s="6">
+        <f t="shared" ref="O72:O77" si="11">10000/3</f>
+        <v>3333.333333</v>
       </c>
       <c r="P72" s="2">
-        <v>1050002.0</v>
-      </c>
-      <c r="Q72" s="2">
-        <f t="shared" si="3"/>
-        <v>2000</v>
+        <f t="shared" ref="P72:P77" si="12">P71+1</f>
+        <v>1050003</v>
+      </c>
+      <c r="Q72" s="6">
+        <f t="shared" ref="Q72:Q77" si="13">10000/3</f>
+        <v>3333.333333</v>
       </c>
       <c r="R72" s="2">
-        <v>1050003.0</v>
-      </c>
-      <c r="S72" s="2">
-        <f t="shared" si="4"/>
-        <v>2000</v>
+        <f t="shared" ref="R72:R77" si="14">R71+1</f>
+        <v>1050004</v>
+      </c>
+      <c r="S72" s="6">
+        <f t="shared" ref="S72:S77" si="15">10000/3</f>
+        <v>3333.333333</v>
       </c>
       <c r="T72" s="2">
-        <v>1050003.0</v>
+        <v>0.0</v>
       </c>
       <c r="U72" s="2">
-        <f t="shared" si="5"/>
-        <v>2000</v>
+        <v>0.0</v>
       </c>
       <c r="V72" s="2">
-        <v>1050005.0</v>
+        <v>0.0</v>
       </c>
       <c r="W72" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X72" s="2">
         <f t="shared" si="6"/>
-        <v>2000</v>
-      </c>
-      <c r="X72" s="2">
-        <f t="shared" si="7"/>
         <v>10000</v>
       </c>
     </row>
     <row r="73">
       <c r="F73" s="2">
-        <f t="shared" si="8"/>
-        <v>9010006</v>
+        <f t="shared" si="7"/>
+        <v>9010008</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>45</v>
       </c>
       <c r="H73" s="2">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="I73" s="2">
         <v>0.0</v>
       </c>
       <c r="K73" s="2">
+        <f t="shared" si="8"/>
+        <v>1070008</v>
+      </c>
+      <c r="L73" s="2">
         <f t="shared" si="9"/>
-        <v>1070006</v>
-      </c>
-      <c r="L73" s="2">
-        <v>1030011.0</v>
+        <v>1030013</v>
       </c>
       <c r="M73" s="2">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="N73" s="2">
-        <v>1050001.0</v>
-      </c>
-      <c r="O73" s="2">
-        <f t="shared" si="2"/>
-        <v>2000</v>
+        <f t="shared" si="10"/>
+        <v>1050003</v>
+      </c>
+      <c r="O73" s="6">
+        <f t="shared" si="11"/>
+        <v>3333.333333</v>
       </c>
       <c r="P73" s="2">
-        <v>1050002.0</v>
-      </c>
-      <c r="Q73" s="2">
-        <f t="shared" si="3"/>
-        <v>2000</v>
+        <f t="shared" si="12"/>
+        <v>1050004</v>
+      </c>
+      <c r="Q73" s="6">
+        <f t="shared" si="13"/>
+        <v>3333.333333</v>
       </c>
       <c r="R73" s="2">
-        <v>1050003.0</v>
-      </c>
-      <c r="S73" s="2">
-        <f t="shared" si="4"/>
-        <v>2000</v>
+        <f t="shared" si="14"/>
+        <v>1050005</v>
+      </c>
+      <c r="S73" s="6">
+        <f t="shared" si="15"/>
+        <v>3333.333333</v>
       </c>
       <c r="T73" s="2">
-        <v>1050003.0</v>
+        <v>0.0</v>
       </c>
       <c r="U73" s="2">
-        <f t="shared" si="5"/>
-        <v>2000</v>
+        <v>0.0</v>
       </c>
       <c r="V73" s="2">
-        <v>1050005.0</v>
+        <v>0.0</v>
       </c>
       <c r="W73" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X73" s="2">
         <f t="shared" si="6"/>
-        <v>2000</v>
-      </c>
-      <c r="X73" s="2">
-        <f t="shared" si="7"/>
         <v>10000</v>
       </c>
     </row>
     <row r="74">
-      <c r="F74" s="2">
+      <c r="K74" s="2">
         <f t="shared" si="8"/>
-        <v>9010007</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H74" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="I74" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="K74" s="2">
+        <v>1070009</v>
+      </c>
+      <c r="L74" s="2">
         <f t="shared" si="9"/>
-        <v>1070007</v>
-      </c>
-      <c r="L74" s="2">
-        <f t="shared" ref="L74:L79" si="10">L73+1</f>
-        <v>1030012</v>
+        <v>1030014</v>
       </c>
       <c r="M74" s="2">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="N74" s="2">
-        <f t="shared" ref="N74:N79" si="11">N73+1</f>
-        <v>1050002</v>
+        <f t="shared" si="10"/>
+        <v>1050004</v>
       </c>
       <c r="O74" s="6">
-        <f t="shared" ref="O74:O79" si="12">10000/3</f>
+        <f t="shared" si="11"/>
         <v>3333.333333</v>
       </c>
       <c r="P74" s="2">
-        <f t="shared" ref="P74:P79" si="13">P73+1</f>
-        <v>1050003</v>
+        <f t="shared" si="12"/>
+        <v>1050005</v>
       </c>
       <c r="Q74" s="6">
-        <f t="shared" ref="Q74:Q79" si="14">10000/3</f>
+        <f t="shared" si="13"/>
         <v>3333.333333</v>
       </c>
       <c r="R74" s="2">
-        <f t="shared" ref="R74:R79" si="15">R73+1</f>
-        <v>1050004</v>
+        <f t="shared" si="14"/>
+        <v>1050006</v>
       </c>
       <c r="S74" s="6">
-        <f t="shared" ref="S74:S79" si="16">10000/3</f>
+        <f t="shared" si="15"/>
         <v>3333.333333</v>
       </c>
       <c r="T74" s="2">
@@ -1389,57 +1530,44 @@
         <v>0.0</v>
       </c>
       <c r="X74" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10000</v>
       </c>
     </row>
     <row r="75">
-      <c r="F75" s="2">
+      <c r="K75" s="2">
         <f t="shared" si="8"/>
-        <v>9010008</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H75" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="I75" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="K75" s="2">
+        <v>1070010</v>
+      </c>
+      <c r="L75" s="2">
         <f t="shared" si="9"/>
-        <v>1070008</v>
-      </c>
-      <c r="L75" s="2">
+        <v>1030015</v>
+      </c>
+      <c r="M75" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="N75" s="2">
         <f t="shared" si="10"/>
-        <v>1030013</v>
-      </c>
-      <c r="M75" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="N75" s="2">
+        <v>1050005</v>
+      </c>
+      <c r="O75" s="6">
         <f t="shared" si="11"/>
-        <v>1050003</v>
-      </c>
-      <c r="O75" s="6">
+        <v>3333.333333</v>
+      </c>
+      <c r="P75" s="2">
         <f t="shared" si="12"/>
+        <v>1050006</v>
+      </c>
+      <c r="Q75" s="6">
+        <f t="shared" si="13"/>
         <v>3333.333333</v>
       </c>
-      <c r="P75" s="2">
-        <f t="shared" si="13"/>
-        <v>1050004</v>
-      </c>
-      <c r="Q75" s="6">
+      <c r="R75" s="2">
         <f t="shared" si="14"/>
-        <v>3333.333333</v>
-      </c>
-      <c r="R75" s="2">
+        <v>1050007</v>
+      </c>
+      <c r="S75" s="6">
         <f t="shared" si="15"/>
-        <v>1050005</v>
-      </c>
-      <c r="S75" s="6">
-        <f t="shared" si="16"/>
         <v>3333.333333</v>
       </c>
       <c r="T75" s="2">
@@ -1455,44 +1583,44 @@
         <v>0.0</v>
       </c>
       <c r="X75" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10000</v>
       </c>
     </row>
     <row r="76">
       <c r="K76" s="2">
+        <f t="shared" si="8"/>
+        <v>1070011</v>
+      </c>
+      <c r="L76" s="2">
         <f t="shared" si="9"/>
-        <v>1070009</v>
-      </c>
-      <c r="L76" s="2">
+        <v>1030016</v>
+      </c>
+      <c r="M76" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="N76" s="2">
         <f t="shared" si="10"/>
-        <v>1030014</v>
-      </c>
-      <c r="M76" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="N76" s="2">
+        <v>1050006</v>
+      </c>
+      <c r="O76" s="6">
         <f t="shared" si="11"/>
-        <v>1050004</v>
-      </c>
-      <c r="O76" s="6">
+        <v>3333.333333</v>
+      </c>
+      <c r="P76" s="2">
         <f t="shared" si="12"/>
+        <v>1050007</v>
+      </c>
+      <c r="Q76" s="6">
+        <f t="shared" si="13"/>
         <v>3333.333333</v>
       </c>
-      <c r="P76" s="2">
-        <f t="shared" si="13"/>
-        <v>1050005</v>
-      </c>
-      <c r="Q76" s="6">
+      <c r="R76" s="2">
         <f t="shared" si="14"/>
-        <v>3333.333333</v>
-      </c>
-      <c r="R76" s="2">
+        <v>1050008</v>
+      </c>
+      <c r="S76" s="6">
         <f t="shared" si="15"/>
-        <v>1050006</v>
-      </c>
-      <c r="S76" s="6">
-        <f t="shared" si="16"/>
         <v>3333.333333</v>
       </c>
       <c r="T76" s="2">
@@ -1508,44 +1636,44 @@
         <v>0.0</v>
       </c>
       <c r="X76" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10000</v>
       </c>
     </row>
     <row r="77">
       <c r="K77" s="2">
+        <f t="shared" si="8"/>
+        <v>1070012</v>
+      </c>
+      <c r="L77" s="2">
         <f t="shared" si="9"/>
-        <v>1070010</v>
-      </c>
-      <c r="L77" s="2">
+        <v>1030017</v>
+      </c>
+      <c r="M77" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="N77" s="2">
         <f t="shared" si="10"/>
-        <v>1030015</v>
-      </c>
-      <c r="M77" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="N77" s="2">
+        <v>1050007</v>
+      </c>
+      <c r="O77" s="6">
         <f t="shared" si="11"/>
-        <v>1050005</v>
-      </c>
-      <c r="O77" s="6">
+        <v>3333.333333</v>
+      </c>
+      <c r="P77" s="2">
         <f t="shared" si="12"/>
+        <v>1050008</v>
+      </c>
+      <c r="Q77" s="6">
+        <f t="shared" si="13"/>
         <v>3333.333333</v>
       </c>
-      <c r="P77" s="2">
-        <f t="shared" si="13"/>
-        <v>1050006</v>
-      </c>
-      <c r="Q77" s="6">
+      <c r="R77" s="2">
         <f t="shared" si="14"/>
-        <v>3333.333333</v>
-      </c>
-      <c r="R77" s="2">
+        <v>1050009</v>
+      </c>
+      <c r="S77" s="6">
         <f t="shared" si="15"/>
-        <v>1050007</v>
-      </c>
-      <c r="S77" s="6">
-        <f t="shared" si="16"/>
         <v>3333.333333</v>
       </c>
       <c r="T77" s="2">
@@ -1561,383 +1689,381 @@
         <v>0.0</v>
       </c>
       <c r="X77" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="78">
-      <c r="K78" s="2">
-        <f t="shared" si="9"/>
-        <v>1070011</v>
-      </c>
-      <c r="L78" s="2">
-        <f t="shared" si="10"/>
-        <v>1030016</v>
-      </c>
-      <c r="M78" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="N78" s="2">
-        <f t="shared" si="11"/>
-        <v>1050006</v>
-      </c>
-      <c r="O78" s="6">
-        <f t="shared" si="12"/>
+    <row r="84">
+      <c r="H84" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M84" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R84" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="F85" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O85" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P85" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T85" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U85" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="F86" s="6">
+        <f t="shared" ref="F86:F108" si="16">(10000/23)</f>
+        <v>434.7826087</v>
+      </c>
+      <c r="H86" s="2">
+        <v>102001.0</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J86" s="2">
+        <v>1030024.0</v>
+      </c>
+      <c r="K86" s="6">
+        <v>10000.0</v>
+      </c>
+      <c r="M86" s="2">
+        <v>103001.0</v>
+      </c>
+      <c r="N86" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O86" s="2">
+        <v>1030001.0</v>
+      </c>
+      <c r="P86" s="6">
+        <f t="shared" ref="P86:P88" si="17">10000/3</f>
         <v>3333.333333</v>
       </c>
-      <c r="P78" s="2">
-        <f t="shared" si="13"/>
-        <v>1050007</v>
-      </c>
-      <c r="Q78" s="6">
-        <f t="shared" si="14"/>
+      <c r="R86" s="2">
+        <v>1021001.0</v>
+      </c>
+      <c r="S86" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T86" s="2">
+        <v>1030028.0</v>
+      </c>
+      <c r="U86" s="6">
+        <f t="shared" ref="U86:U87" si="18">10000/2</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="F87" s="6">
+        <f t="shared" si="16"/>
+        <v>434.7826087</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
+      <c r="K87" s="8">
+        <f>SUM(K86)</f>
+        <v>10000</v>
+      </c>
+      <c r="M87" s="2">
+        <v>103001.0</v>
+      </c>
+      <c r="N87" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O87" s="2">
+        <f t="shared" ref="O87:O88" si="19">O86+1</f>
+        <v>1030002</v>
+      </c>
+      <c r="P87" s="6">
+        <f t="shared" si="17"/>
         <v>3333.333333</v>
       </c>
-      <c r="R78" s="2">
-        <f t="shared" si="15"/>
-        <v>1050008</v>
-      </c>
-      <c r="S78" s="6">
-        <f t="shared" si="16"/>
-        <v>3333.333333</v>
-      </c>
-      <c r="T78" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="U78" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="V78" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="W78" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="X78" s="2">
-        <f t="shared" si="7"/>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="K79" s="2">
-        <f t="shared" si="9"/>
-        <v>1070012</v>
-      </c>
-      <c r="L79" s="2">
-        <f t="shared" si="10"/>
-        <v>1030017</v>
-      </c>
-      <c r="M79" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="N79" s="2">
-        <f t="shared" si="11"/>
-        <v>1050007</v>
-      </c>
-      <c r="O79" s="6">
-        <f t="shared" si="12"/>
-        <v>3333.333333</v>
-      </c>
-      <c r="P79" s="2">
-        <f t="shared" si="13"/>
-        <v>1050008</v>
-      </c>
-      <c r="Q79" s="6">
-        <f t="shared" si="14"/>
-        <v>3333.333333</v>
-      </c>
-      <c r="R79" s="2">
-        <f t="shared" si="15"/>
-        <v>1050009</v>
-      </c>
-      <c r="S79" s="6">
-        <f t="shared" si="16"/>
-        <v>3333.333333</v>
-      </c>
-      <c r="T79" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="U79" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="V79" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="W79" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="X79" s="2">
-        <f t="shared" si="7"/>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="H86" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M86" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R86" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="F87" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J87" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K87" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M87" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N87" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O87" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P87" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="R87" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S87" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T87" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="U87" s="1" t="s">
-        <v>46</v>
+      <c r="R87" s="2">
+        <v>1021001.0</v>
+      </c>
+      <c r="S87" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T87" s="2">
+        <v>1030029.0</v>
+      </c>
+      <c r="U87" s="6">
+        <f t="shared" si="18"/>
+        <v>5000</v>
       </c>
     </row>
     <row r="88">
       <c r="F88" s="6">
-        <f t="shared" ref="F88:F110" si="17">(10000/23)</f>
-        <v>434.7826087</v>
-      </c>
-      <c r="H88" s="2">
-        <v>102001.0</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J88" s="2">
-        <v>1030024.0</v>
-      </c>
-      <c r="K88" s="6">
-        <v>10000.0</v>
+        <f t="shared" si="16"/>
+        <v>434.7826087</v>
       </c>
       <c r="M88" s="2">
         <v>103001.0</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O88" s="2">
-        <v>1030001.0</v>
+        <f t="shared" si="19"/>
+        <v>1030003</v>
       </c>
       <c r="P88" s="6">
-        <f t="shared" ref="P88:P90" si="18">10000/3</f>
+        <f t="shared" si="17"/>
         <v>3333.333333</v>
       </c>
-      <c r="R88" s="2">
-        <v>1021001.0</v>
-      </c>
-      <c r="S88" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="T88" s="2">
-        <v>1030028.0</v>
-      </c>
-      <c r="U88" s="6">
-        <f t="shared" ref="U88:U89" si="19">10000/2</f>
-        <v>5000</v>
+      <c r="R88" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="S88" s="7"/>
+      <c r="T88" s="7"/>
+      <c r="U88" s="8">
+        <f>SUM(U86:U87)</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="89">
       <c r="F89" s="6">
-        <f t="shared" si="17"/>
-        <v>434.7826087</v>
-      </c>
-      <c r="H89" s="7" t="s">
+        <f t="shared" si="16"/>
+        <v>434.7826087</v>
+      </c>
+      <c r="M89" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I89" s="7"/>
-      <c r="J89" s="7"/>
-      <c r="K89" s="8">
-        <f>SUM(K88)</f>
+      <c r="N89" s="7"/>
+      <c r="O89" s="7"/>
+      <c r="P89" s="8">
+        <f>SUM(P86:P88)</f>
         <v>10000</v>
-      </c>
-      <c r="M89" s="2">
-        <v>103001.0</v>
-      </c>
-      <c r="N89" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O89" s="2">
-        <f t="shared" ref="O89:O90" si="20">O88+1</f>
-        <v>1030002</v>
-      </c>
-      <c r="P89" s="6">
-        <f t="shared" si="18"/>
-        <v>3333.333333</v>
-      </c>
-      <c r="R89" s="2">
-        <v>1021001.0</v>
-      </c>
-      <c r="S89" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="T89" s="2">
-        <v>1030029.0</v>
-      </c>
-      <c r="U89" s="6">
-        <f t="shared" si="19"/>
-        <v>5000</v>
       </c>
     </row>
     <row r="90">
       <c r="F90" s="6">
-        <f t="shared" si="17"/>
-        <v>434.7826087</v>
-      </c>
-      <c r="M90" s="2">
-        <v>103001.0</v>
-      </c>
-      <c r="N90" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O90" s="2">
-        <f t="shared" si="20"/>
-        <v>1030003</v>
-      </c>
-      <c r="P90" s="6">
-        <f t="shared" si="18"/>
-        <v>3333.333333</v>
-      </c>
-      <c r="R90" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="S90" s="7"/>
-      <c r="T90" s="7"/>
-      <c r="U90" s="8">
-        <f>SUM(U88:U89)</f>
-        <v>10000</v>
+        <f t="shared" si="16"/>
+        <v>434.7826087</v>
       </c>
     </row>
     <row r="91">
       <c r="F91" s="6">
-        <f t="shared" si="17"/>
-        <v>434.7826087</v>
-      </c>
-      <c r="M91" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="N91" s="7"/>
-      <c r="O91" s="7"/>
-      <c r="P91" s="8">
-        <f>SUM(P88:P90)</f>
-        <v>10000</v>
+        <f t="shared" si="16"/>
+        <v>434.7826087</v>
       </c>
     </row>
     <row r="92">
       <c r="F92" s="6">
-        <f t="shared" si="17"/>
-        <v>434.7826087</v>
+        <f t="shared" si="16"/>
+        <v>434.7826087</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V92" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="93">
       <c r="F93" s="6">
-        <f t="shared" si="17"/>
-        <v>434.7826087</v>
+        <f t="shared" si="16"/>
+        <v>434.7826087</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N93" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O93" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P93" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q93" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R93" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S93" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T93" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U93" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V93" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="94">
       <c r="F94" s="6">
-        <f t="shared" si="17"/>
-        <v>434.7826087</v>
-      </c>
-      <c r="H94" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J94" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="V94" s="3" t="s">
-        <v>50</v>
+        <f t="shared" si="16"/>
+        <v>434.7826087</v>
+      </c>
+      <c r="H94" s="2">
+        <v>2010001.0</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K94" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="L94" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="M94" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N94" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O94" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="P94" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q94" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="R94" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="S94" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T94" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="U94" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="V94" s="2">
+        <v>8.0</v>
       </c>
     </row>
     <row r="95">
       <c r="F95" s="6">
-        <f t="shared" si="17"/>
-        <v>434.7826087</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J95" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K95" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L95" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M95" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N95" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O95" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P95" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q95" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="R95" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S95" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T95" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U95" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="V95" s="1" t="s">
-        <v>64</v>
+        <f t="shared" si="16"/>
+        <v>434.7826087</v>
+      </c>
+      <c r="H95" s="2">
+        <f t="shared" ref="H95:H100" si="20">H94+1</f>
+        <v>2010002</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K95" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="L95" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="M95" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N95" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="O95" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="P95" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q95" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="R95" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="S95" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T95" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="U95" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="V95" s="2">
+        <v>8.0</v>
       </c>
     </row>
     <row r="96">
       <c r="F96" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>434.7826087</v>
       </c>
       <c r="H96" s="2">
-        <v>2010001.0</v>
+        <f t="shared" si="20"/>
+        <v>2010003</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>65</v>
@@ -1984,12 +2110,12 @@
     </row>
     <row r="97">
       <c r="F97" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>434.7826087</v>
       </c>
       <c r="H97" s="2">
-        <f t="shared" ref="H97:H102" si="21">H96+1</f>
-        <v>2010002</v>
+        <f t="shared" si="20"/>
+        <v>2010004</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>65</v>
@@ -1998,34 +2124,34 @@
         <v>66</v>
       </c>
       <c r="K97" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="L97" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M97" s="2" t="s">
         <v>67</v>
       </c>
       <c r="N97" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O97" s="2">
         <v>3.0</v>
-      </c>
-      <c r="O97" s="2">
-        <v>5.0</v>
       </c>
       <c r="P97" s="2" t="s">
         <v>68</v>
       </c>
       <c r="Q97" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="R97" s="2">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="S97" s="2" t="s">
         <v>69</v>
       </c>
       <c r="T97" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="U97" s="2">
         <v>3.0</v>
@@ -2036,12 +2162,12 @@
     </row>
     <row r="98">
       <c r="F98" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>434.7826087</v>
       </c>
       <c r="H98" s="2">
-        <f t="shared" si="21"/>
-        <v>2010003</v>
+        <f t="shared" si="20"/>
+        <v>2010005</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>65</v>
@@ -2088,12 +2214,12 @@
     </row>
     <row r="99">
       <c r="F99" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>434.7826087</v>
       </c>
       <c r="H99" s="2">
-        <f t="shared" si="21"/>
-        <v>2010004</v>
+        <f t="shared" si="20"/>
+        <v>2010006</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>65</v>
@@ -2140,12 +2266,12 @@
     </row>
     <row r="100">
       <c r="F100" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>434.7826087</v>
       </c>
       <c r="H100" s="2">
-        <f t="shared" si="21"/>
-        <v>2010005</v>
+        <f t="shared" si="20"/>
+        <v>2010007</v>
       </c>
       <c r="I100" s="2" t="s">
         <v>65</v>
@@ -2192,879 +2318,775 @@
     </row>
     <row r="101">
       <c r="F101" s="6">
-        <f t="shared" si="17"/>
-        <v>434.7826087</v>
-      </c>
-      <c r="H101" s="2">
-        <f t="shared" si="21"/>
-        <v>2010006</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K101" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="L101" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="M101" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N101" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="O101" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="P101" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q101" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="R101" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="S101" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="T101" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="U101" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="V101" s="2">
-        <v>8.0</v>
+        <f t="shared" si="16"/>
+        <v>434.7826087</v>
       </c>
     </row>
     <row r="102">
       <c r="F102" s="6">
-        <f t="shared" si="17"/>
-        <v>434.7826087</v>
-      </c>
-      <c r="H102" s="2">
-        <f t="shared" si="21"/>
-        <v>2010007</v>
-      </c>
-      <c r="I102" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J102" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K102" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="L102" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="M102" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N102" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="O102" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="P102" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q102" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="R102" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="S102" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="T102" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="U102" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="V102" s="2">
-        <v>8.0</v>
+        <f t="shared" si="16"/>
+        <v>434.7826087</v>
       </c>
     </row>
     <row r="103">
       <c r="F103" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="104">
       <c r="F104" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="105">
       <c r="F105" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="106">
       <c r="F106" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="107">
       <c r="F107" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="108">
       <c r="F108" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="109">
-      <c r="F109" s="6">
-        <f t="shared" si="17"/>
-        <v>434.7826087</v>
+      <c r="F109" s="8">
+        <f>SUM(F86:F108)</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="110">
       <c r="F110" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="F110:F132" si="21">(10000/23)</f>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="111">
-      <c r="F111" s="8">
-        <f>SUM(F88:F110)</f>
-        <v>10000</v>
+      <c r="F111" s="6">
+        <f t="shared" si="21"/>
+        <v>434.7826087</v>
       </c>
     </row>
     <row r="112">
       <c r="F112" s="6">
-        <f t="shared" ref="F112:F134" si="22">(10000/23)</f>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="113">
       <c r="F113" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="114">
       <c r="F114" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="115">
       <c r="F115" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="116">
       <c r="F116" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="117">
       <c r="F117" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="118">
       <c r="F118" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="119">
       <c r="F119" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="120">
       <c r="F120" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="121">
       <c r="F121" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="122">
       <c r="F122" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="123">
       <c r="F123" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="124">
       <c r="F124" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="125">
       <c r="F125" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="126">
       <c r="F126" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="127">
       <c r="F127" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="128">
       <c r="F128" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="129">
       <c r="F129" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="130">
       <c r="F130" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="131">
       <c r="F131" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="132">
       <c r="F132" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="133">
-      <c r="F133" s="6">
-        <f t="shared" si="22"/>
-        <v>434.7826087</v>
+      <c r="F133" s="8">
+        <f>SUM(F110:F132)</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="134">
       <c r="F134" s="6">
+        <f t="shared" ref="F134:F156" si="22">(10000/23)</f>
+        <v>434.7826087</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="F135" s="6">
         <f t="shared" si="22"/>
         <v>434.7826087</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="F135" s="8">
-        <f>SUM(F112:F134)</f>
-        <v>10000</v>
       </c>
     </row>
     <row r="136">
       <c r="F136" s="6">
-        <f t="shared" ref="F136:F158" si="23">(10000/23)</f>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="137">
       <c r="F137" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="138">
       <c r="F138" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="139">
       <c r="F139" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="140">
       <c r="F140" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="141">
       <c r="F141" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="142">
       <c r="F142" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="143">
       <c r="F143" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="144">
       <c r="F144" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="145">
       <c r="F145" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="146">
       <c r="F146" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="147">
       <c r="F147" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="148">
       <c r="F148" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="149">
       <c r="F149" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="150">
       <c r="F150" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="151">
       <c r="F151" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="152">
       <c r="F152" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="153">
       <c r="F153" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="154">
       <c r="F154" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="155">
       <c r="F155" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="156">
       <c r="F156" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="157">
-      <c r="F157" s="6">
-        <f t="shared" si="23"/>
-        <v>434.7826087</v>
+      <c r="F157" s="8">
+        <f>SUM(F134:F156)</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="158">
       <c r="F158" s="6">
+        <f t="shared" ref="F158:F180" si="23">(10000/23)</f>
+        <v>434.7826087</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="F159" s="6">
         <f t="shared" si="23"/>
         <v>434.7826087</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="F159" s="8">
-        <f>SUM(F136:F158)</f>
-        <v>10000</v>
       </c>
     </row>
     <row r="160">
       <c r="F160" s="6">
-        <f t="shared" ref="F160:F182" si="24">(10000/23)</f>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="161">
       <c r="F161" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="162">
       <c r="F162" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="163">
       <c r="F163" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="164">
       <c r="F164" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="165">
       <c r="F165" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="166">
       <c r="F166" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="167">
       <c r="F167" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="168">
       <c r="F168" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="169">
       <c r="F169" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="170">
       <c r="F170" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="171">
       <c r="F171" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="172">
       <c r="F172" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="173">
       <c r="F173" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="174">
       <c r="F174" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="175">
       <c r="F175" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="176">
       <c r="F176" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="177">
       <c r="F177" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="178">
       <c r="F178" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="179">
       <c r="F179" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="180">
       <c r="F180" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="181">
-      <c r="F181" s="6">
-        <f t="shared" si="24"/>
-        <v>434.7826087</v>
+      <c r="F181" s="8">
+        <f>SUM(F158:F180)</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="182">
       <c r="F182" s="6">
+        <f t="shared" ref="F182:F204" si="24">(10000/23)</f>
+        <v>434.7826087</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="F183" s="6">
         <f t="shared" si="24"/>
         <v>434.7826087</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="F183" s="8">
-        <f>SUM(F160:F182)</f>
-        <v>10000</v>
       </c>
     </row>
     <row r="184">
       <c r="F184" s="6">
-        <f t="shared" ref="F184:F206" si="25">(10000/23)</f>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="185">
       <c r="F185" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="186">
       <c r="F186" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="187">
       <c r="F187" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="188">
       <c r="F188" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="189">
       <c r="F189" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="190">
       <c r="F190" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="191">
       <c r="F191" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="192">
       <c r="F192" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="193">
       <c r="F193" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="194">
       <c r="F194" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="195">
       <c r="F195" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="196">
       <c r="F196" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="197">
       <c r="F197" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="198">
       <c r="F198" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="199">
       <c r="F199" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="200">
       <c r="F200" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="201">
       <c r="F201" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="202">
       <c r="F202" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="203">
       <c r="F203" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="204">
       <c r="F204" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="205">
-      <c r="F205" s="6">
-        <f t="shared" si="25"/>
-        <v>434.7826087</v>
+      <c r="F205" s="8">
+        <f>SUM(F182:F204)</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="206">
       <c r="F206" s="6">
+        <f t="shared" ref="F206:F228" si="25">(10000/23)</f>
+        <v>434.7826087</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="F207" s="6">
         <f t="shared" si="25"/>
         <v>434.7826087</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="F207" s="8">
-        <f>SUM(F184:F206)</f>
-        <v>10000</v>
       </c>
     </row>
     <row r="208">
       <c r="F208" s="6">
-        <f t="shared" ref="F208:F230" si="26">(10000/23)</f>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="209">
       <c r="F209" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="210">
       <c r="F210" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="211">
       <c r="F211" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="212">
       <c r="F212" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="213">
       <c r="F213" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="214">
       <c r="F214" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="215">
       <c r="F215" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="216">
       <c r="F216" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="217">
       <c r="F217" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="218">
       <c r="F218" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="219">
       <c r="F219" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="220">
       <c r="F220" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="221">
       <c r="F221" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="222">
       <c r="F222" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="223">
       <c r="F223" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="224">
       <c r="F224" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="225">
       <c r="F225" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="226">
       <c r="F226" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="227">
       <c r="F227" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="228">
       <c r="F228" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>434.7826087</v>
       </c>
     </row>
     <row r="229">
-      <c r="F229" s="6">
-        <f t="shared" si="26"/>
-        <v>434.7826087</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="F230" s="6">
-        <f t="shared" si="26"/>
-        <v>434.7826087</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="F231" s="8">
-        <f>SUM(F208:F230)</f>
+      <c r="F229" s="8">
+        <f>SUM(F206:F228)</f>
         <v>10000</v>
       </c>
     </row>
@@ -3073,7 +3095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3088,12 +3110,12 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>